<commit_message>
Day 3 | 31-07-2024
</commit_message>
<xml_diff>
--- a/SERVICE_REMINDER_FUNCTIONALITY_TEST_CASES.xlsx
+++ b/SERVICE_REMINDER_FUNCTIONALITY_TEST_CASES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TELOSA\TELOSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E840F5-E1FD-4B78-867A-5A45ACCB7B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5757D56A-702E-4260-9D63-C0B0E09E92F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="525" xr2:uid="{84634E0E-FAA6-44D9-AD62-EF3D872C32E8}"/>
   </bookViews>
@@ -161,9 +161,6 @@
     <t>TEL_SR_11</t>
   </si>
   <si>
-    <t>To validate the send after field using invalid data</t>
-  </si>
-  <si>
     <t>Days : @abc</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
   </si>
   <si>
     <t xml:space="preserve">The did not allow user to type the non numerical characters </t>
-  </si>
-  <si>
-    <t>To validate the send after field using blank input</t>
   </si>
   <si>
     <t xml:space="preserve">Days : </t>
@@ -195,16 +189,10 @@
 • Press Plus Button </t>
   </si>
   <si>
-    <t xml:space="preserve">To validate the Plus button for send after days field </t>
-  </si>
-  <si>
     <t xml:space="preserve">The system should increase the days count </t>
   </si>
   <si>
     <t xml:space="preserve">The system increased the days count </t>
-  </si>
-  <si>
-    <t xml:space="preserve">To validate the Minus button for send after days field </t>
   </si>
   <si>
     <t xml:space="preserve">• Login to System 
@@ -280,9 +268,6 @@
   </si>
   <si>
     <t xml:space="preserve">The system should show the all templates available to select </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The system should showed the all templates available to select </t>
   </si>
   <si>
     <t>User should be able to select the templates from drop down</t>
@@ -663,9 +648,6 @@
 The subsequent SR will follow the updated SR interval of 15 days. This places the next SR on 20 January (5 January + 15 days).</t>
   </si>
   <si>
-    <t xml:space="preserve">To validate the send after ((days) field using valid data </t>
-  </si>
-  <si>
     <t xml:space="preserve">To validate that service reminder is triggered as per the date of the second visit if the user visits before the first service reminder is triggered </t>
   </si>
   <si>
@@ -673,6 +655,24 @@
   </si>
   <si>
     <t xml:space="preserve">PASSWORD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To validate the send after (Days) field using valid data </t>
+  </si>
+  <si>
+    <t>To validate the send after (Days) field using invalid data</t>
+  </si>
+  <si>
+    <t>To validate the  send after (Days) field using blank input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To validate the Plus button for  send after (Days) field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To validate the Minus button for send after (Days) field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system should did not show the sms template  </t>
   </si>
 </sst>
 </file>
@@ -810,6 +810,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -818,12 +824,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1143,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098F42E8-0B3A-4AE3-B7BA-B0105D4B8AAF}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1154,7 +1154,7 @@
     <col min="3" max="3" width="14.44140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" style="3" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="36.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="36.77734375" style="3" customWidth="1"/>
     <col min="7" max="7" width="15.44140625" style="3" customWidth="1"/>
     <col min="8" max="8" width="10" style="3" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
@@ -1162,17 +1162,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1204,39 +1204,39 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C5" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1263,22 +1263,22 @@
         <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>12</v>
@@ -1292,25 +1292,25 @@
         <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="I7" s="4">
         <v>45504</v>
@@ -1321,22 +1321,22 @@
         <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>12</v>
@@ -1350,22 +1350,22 @@
         <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>12</v>
@@ -1379,22 +1379,22 @@
         <v>33</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>12</v>
@@ -1408,22 +1408,22 @@
         <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>12</v>
@@ -1437,22 +1437,22 @@
         <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>12</v>
@@ -1466,22 +1466,22 @@
         <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>12</v>
@@ -1495,9 +1495,9 @@
         <v>37</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1507,13 +1507,13 @@
         <v>8</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>74</v>
+        <v>176</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="I14" s="4">
         <v>45504</v>
@@ -1524,9 +1524,9 @@
         <v>38</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -1536,10 +1536,10 @@
         <v>8</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>12</v>
@@ -1550,25 +1550,25 @@
     </row>
     <row r="16" spans="1:9" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>12</v>
@@ -1579,25 +1579,25 @@
     </row>
     <row r="17" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>12</v>
@@ -1608,25 +1608,25 @@
     </row>
     <row r="18" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="F18" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>12</v>
@@ -1637,25 +1637,25 @@
     </row>
     <row r="19" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>12</v>
@@ -1666,22 +1666,22 @@
     </row>
     <row r="20" spans="1:9" ht="106.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C20" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1689,12 +1689,12 @@
     </row>
     <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -1704,7 +1704,7 @@
         <v>8</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1712,12 +1712,12 @@
     </row>
     <row r="22" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C22" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -1727,7 +1727,7 @@
         <v>8</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1735,12 +1735,12 @@
     </row>
     <row r="23" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1750,7 +1750,7 @@
         <v>8</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -1758,22 +1758,22 @@
     </row>
     <row r="24" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -1781,25 +1781,25 @@
     </row>
     <row r="25" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>12</v>
@@ -1810,25 +1810,25 @@
     </row>
     <row r="26" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C26" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>12</v>
@@ -1839,22 +1839,22 @@
     </row>
     <row r="27" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C27" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1862,22 +1862,22 @@
     </row>
     <row r="28" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C28" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1885,22 +1885,22 @@
     </row>
     <row r="29" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C29" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1908,22 +1908,22 @@
     </row>
     <row r="30" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -1931,22 +1931,22 @@
     </row>
     <row r="31" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C31" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -1954,22 +1954,22 @@
     </row>
     <row r="32" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C32" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -1977,22 +1977,22 @@
     </row>
     <row r="33" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C33" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -2000,22 +2000,22 @@
     </row>
     <row r="34" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C34" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -2023,22 +2023,22 @@
     </row>
     <row r="35" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C35" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -2046,22 +2046,22 @@
     </row>
     <row r="36" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C36" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -2069,22 +2069,22 @@
     </row>
     <row r="37" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C37" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -2092,22 +2092,22 @@
     </row>
     <row r="38" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C38" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -2115,22 +2115,22 @@
     </row>
     <row r="39" spans="1:9" ht="183.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C39" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -2138,22 +2138,22 @@
     </row>
     <row r="40" spans="1:9" ht="199.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C40" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -2208,10 +2208,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2224,7 +2224,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2238,31 +2238,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -2289,7 +2289,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5">
         <f>B5/A5*100</f>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="E5" s="5">
         <f>C5/A5*100</f>
-        <v>0</v>
+        <v>2.7777777777777777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>